<commit_message>
Now plotting LightYield vs dose
</commit_message>
<xml_diff>
--- a/RochesterAnalysis/Raddam_Data.xlsx
+++ b/RochesterAnalysis/Raddam_Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="38">
   <si>
     <t xml:space="preserve">TileName</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t xml:space="preserve">10x10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">N2</t>
@@ -289,8 +292,8 @@
   </sheetPr>
   <dimension ref="A1:S99"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -381,7 +384,9 @@
       <c r="E2" s="3" t="n">
         <v>45</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="G2" s="6" t="n">
         <v>144</v>
       </c>
@@ -437,7 +442,9 @@
       <c r="E3" s="5" t="n">
         <v>3.5</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="G3" s="6" t="n">
         <v>20800</v>
       </c>
@@ -493,7 +500,9 @@
       <c r="E4" s="3" t="n">
         <v>45</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="G4" s="6" t="n">
         <v>582</v>
       </c>
@@ -528,7 +537,7 @@
         <v>45</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G5" s="6" t="n">
         <v>144</v>
@@ -555,14 +564,14 @@
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G6" s="8"/>
       <c r="J6" s="0" t="n">
@@ -587,13 +596,13 @@
         <v>11</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1.7</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G7" s="8"/>
       <c r="J7" s="0" t="n">
@@ -618,7 +627,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5" t="n">
         <v>1.7</v>
@@ -626,7 +635,9 @@
       <c r="E8" s="5" t="n">
         <v>3.5</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="G8" s="6" t="n">
         <v>19704</v>
       </c>
@@ -674,7 +685,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" s="5" t="n">
         <v>0.1</v>
@@ -682,7 +693,9 @@
       <c r="E9" s="5" t="n">
         <v>3.5</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="G9" s="6" t="n">
         <v>20800</v>
       </c>
@@ -708,7 +721,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3" t="n">
         <v>0.1</v>
@@ -716,7 +729,9 @@
       <c r="E10" s="3" t="n">
         <v>45</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="G10" s="6" t="n">
         <v>144</v>
       </c>
@@ -742,7 +757,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D11" s="3" t="n">
         <v>0.3</v>
@@ -776,14 +791,14 @@
         <v>12</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" s="3" t="n">
         <v>1.7</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G12" s="8"/>
       <c r="M12" s="7"/>
@@ -796,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13" s="5" t="n">
         <v>10</v>
@@ -804,7 +819,9 @@
       <c r="E13" s="5" t="n">
         <v>3.5</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="G13" s="6" t="n">
         <v>20700</v>
       </c>
@@ -852,7 +869,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D14" s="5" t="n">
         <v>10</v>
@@ -861,7 +878,7 @@
         <v>3.5</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G14" s="6" t="n">
         <v>20700</v>
@@ -888,7 +905,7 @@
         <v>4</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D15" s="3" t="n">
         <v>1.7</v>
@@ -897,7 +914,7 @@
         <v>3.5</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G15" s="6" t="n">
         <v>20800</v>
@@ -930,7 +947,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D16" s="5" t="n">
         <v>0.1</v>
@@ -939,7 +956,7 @@
         <v>45</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G16" s="6" t="n">
         <v>144</v>
@@ -966,7 +983,7 @@
         <v>9</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D17" s="5" t="n">
         <v>0.3</v>
@@ -975,7 +992,7 @@
         <v>45</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G17" s="6" t="n">
         <v>582</v>
@@ -1002,14 +1019,14 @@
         <v>30</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D18" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G18" s="8"/>
       <c r="J18" s="0" t="n">
@@ -1034,14 +1051,14 @@
         <v>31</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D19" s="3" t="n">
         <v>1.7</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G19" s="8"/>
       <c r="J19" s="0" t="n">
@@ -1066,13 +1083,15 @@
         <v>32</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D20" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="G20" s="8"/>
       <c r="J20" s="0" t="n">
         <v>14.082</v>
@@ -1096,13 +1115,15 @@
         <v>33</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D21" s="3" t="n">
         <v>1.7</v>
       </c>
       <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="G21" s="8"/>
       <c r="M21" s="7"/>
     </row>
@@ -1114,14 +1135,14 @@
         <v>34</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D22" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G22" s="8"/>
       <c r="J22" s="0" t="n">
@@ -1146,14 +1167,14 @@
         <v>35</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D23" s="5" t="n">
         <v>1.7</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G23" s="8"/>
       <c r="M23" s="7"/>
@@ -1166,14 +1187,14 @@
         <v>36</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D24" s="5" t="n">
         <v>0.1</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G24" s="8"/>
       <c r="J24" s="0" t="n">
@@ -1723,7 +1744,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B84" s="8"/>
       <c r="C84" s="8"/>
@@ -1734,13 +1755,13 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B85" s="10" t="n">
         <v>4</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D85" s="10" t="n">
         <v>1.7</v>
@@ -1749,19 +1770,19 @@
         <v>3.5</v>
       </c>
       <c r="F85" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G85" s="8"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B86" s="10" t="n">
         <v>3</v>
       </c>
       <c r="C86" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D86" s="10" t="n">
         <v>1.7</v>
@@ -1774,13 +1795,13 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B87" s="10" t="n">
         <v>2</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D87" s="10" t="n">
         <v>10</v>
@@ -1789,7 +1810,7 @@
         <v>3.5</v>
       </c>
       <c r="F87" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G87" s="8"/>
     </row>
@@ -1822,7 +1843,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B91" s="8"/>
       <c r="C91" s="8"/>
@@ -1833,13 +1854,13 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B92" s="10" t="n">
         <v>3</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D92" s="10" t="n">
         <v>1.7</v>
@@ -1852,7 +1873,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
@@ -1863,7 +1884,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
@@ -1874,13 +1895,13 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B95" s="10" t="n">
         <v>2</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D95" s="10" t="n">
         <v>10</v>
@@ -1889,13 +1910,13 @@
         <v>3.5</v>
       </c>
       <c r="F95" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G95" s="8"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B96" s="8"/>
       <c r="C96" s="8"/>
@@ -1906,13 +1927,13 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B97" s="10" t="n">
         <v>2</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D97" s="10" t="n">
         <v>10</v>
@@ -1921,13 +1942,13 @@
         <v>3.5</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G97" s="8"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
@@ -1938,7 +1959,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B99" s="8"/>
       <c r="C99" s="8"/>

</xml_diff>